<commit_message>
add new symptom questions and map new JSON to correct place
</commit_message>
<xml_diff>
--- a/survey-GUI/files/survey-choices.xlsx
+++ b/survey-GUI/files/survey-choices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10392" windowWidth="19392" xWindow="-96" yWindow="-96"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7374" windowWidth="14400" xWindow="0" yWindow="2562"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
@@ -376,16 +376,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F174"/>
+  <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="18.62890625"/>
-    <col customWidth="1" max="2" min="2" width="15.1015625"/>
+    <col customWidth="1" max="2" min="2" width="17.62890625"/>
     <col customWidth="1" max="3" min="3" width="30.89453125"/>
   </cols>
   <sheetData>
@@ -2733,90 +2733,192 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>who_live_with</t>
+          <t>has_facial_swelling</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Who do you live with?</t>
+          <t>Do you have facial swelling?</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>who_sharefood_with</t>
+          <t>has_muscle_fatigue</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Who do you share food with?</t>
+          <t>Do you have muscle fatigue?</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>who_work_with</t>
+          <t>has_vomiting</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Who do you work with?</t>
+          <t>Are you vomiting?</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>new_section</t>
+          <t>select_one yes_no_3</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>has_cough</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Do you have a cough?</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_4</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>questions</t>
+          <t>has_meningitis</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Please, do you have any question for me?</t>
+          <t>Do you have meningitis?</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
+          <t>select_one yes_no_5</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>has_hypertension</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Do you have hypertension?</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
+        <is>
           <t>text</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>who_live_with</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Who do you live with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>who_sharefood_with</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Who do you share food with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>who_work_with</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Who do you work with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
+        <is>
+          <t>new_section</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>questions</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Please, do you have any question for me?</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="C174" t="inlineStr">
+      <c r="C180" t="inlineStr">
         <is>
           <t>Include any notes about this interview</t>
         </is>

</xml_diff>

<commit_message>
update questions to add GPS type
</commit_message>
<xml_diff>
--- a/survey-GUI/files/survey-choices.xlsx
+++ b/survey-GUI/files/survey-choices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10392" windowWidth="19392" xWindow="-96" yWindow="-96"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10536" windowWidth="19392" xWindow="-96" yWindow="-96"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
@@ -376,10 +376,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F174"/>
+  <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -577,7 +577,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>gps_coord</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2733,90 +2733,192 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>who_live_with</t>
+          <t>has_facial_swelling</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Who do you live with?</t>
+          <t>Do you have facial swelling?</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>who_sharefood_with</t>
+          <t>has_muscle_fatigue</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Who do you share food with?</t>
+          <t>Do you have muscle fatigue?</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>who_work_with</t>
+          <t>has_vomiting</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Who do you work with?</t>
+          <t>Are you vomiting?</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>new_section</t>
+          <t>select_one yes_no_2</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>has_cough</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Do you have a cough?</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one yes_no_2</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>questions</t>
+          <t>has_meningitis</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Please, do you have any question for me?</t>
+          <t>Do you have meningitis?</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
+          <t>select_one yes_no_2</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>has_hypertension</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Do you have hypertension?</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
+        <is>
           <t>text</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>who_live_with</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Who do you live with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>who_sharefood_with</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Who do you share food with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>who_work_with</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Who do you work with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
+        <is>
+          <t>new_section</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>questions</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Please, do you have any question for me?</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="C174" t="inlineStr">
+      <c r="C180" t="inlineStr">
         <is>
           <t>Include any notes about this interview</t>
         </is>

</xml_diff>